<commit_message>
update the base function
</commit_message>
<xml_diff>
--- a/nft_net_hub/info/NFT1000_download_info.xlsx
+++ b/nft_net_hub/info/NFT1000_download_info.xlsx
@@ -62,7 +62,7 @@
     <t>BoredApeYachtClub</t>
   </si>
   <si>
-    <t/>
+    <t>nan</t>
   </si>
   <si>
     <t>CRYPTOPUNKS</t>
@@ -4055,17 +4055,11 @@
   <sheetPr/>
   <dimension ref="A1:J1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="2" width="45.5925925925926" customWidth="1"/>
-    <col min="3" max="3" width="21.9166666666667" customWidth="1"/>
-    <col min="4" max="4" width="16.9259259259259" customWidth="1"/>
-    <col min="9" max="9" width="28.0462962962963" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">

</xml_diff>